<commit_message>
collect goal condition information
</commit_message>
<xml_diff>
--- a/tests/plus_selectif_min.xlsx
+++ b/tests/plus_selectif_min.xlsx
@@ -31,8 +31,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -112,12 +113,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,7 +139,18 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <name val="Arial"/>
@@ -234,7 +250,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -263,13 +279,13 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1" t="e">
+      <c r="C4" s="2" t="e">
         <f aca="false">selectif(777,D1&gt;E1,B1-A1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -289,12 +305,17 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>D1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>666</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>0</formula>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"bla-bla"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add condition cell to used cell
</commit_message>
<xml_diff>
--- a/tests/plus_selectif_min.xlsx
+++ b/tests/plus_selectif_min.xlsx
@@ -250,7 +250,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,7 +285,9 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>